<commit_message>
add Transformer Calculation method
</commit_message>
<xml_diff>
--- a/CNIntelligibility/intelligibility_bm25.xlsx
+++ b/CNIntelligibility/intelligibility_bm25.xlsx
@@ -563,2371 +563,2371 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>01-21377035</t>
+          <t>01-22377201</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.5785444914533868</v>
+        <v>-1.702596318852223</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1019153983063911</v>
+        <v>-0.2360187881952261</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>-0.1385912804396006</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.0278959254474382</v>
+        <v>-0.5117493724383535</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.620579224153986</v>
+        <v>-2.115577992495515</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.0319395234075526</v>
+        <v>-0.0896268045153323</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>-0.2278409824152689</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.0165060596714404</v>
+        <v>-0.1217469991543331</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.0295852557432739</v>
+        <v>-0.1576612463016983</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.0964724275591768</v>
+        <v>-0.2988254462258066</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.08640857905064341</v>
+        <v>-0.0945356216961333</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.0239938486556044</v>
+        <v>-0.1720376091927651</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.0254071466052445</v>
+        <v>-0.3190501642071545</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.1027925673999881</v>
+        <v>-0.1696460197321566</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.0295317570947726</v>
+        <v>-0.2689804632944088</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>-0.1525340644598688</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.0309507290852711</v>
+        <v>-0.3436563829699597</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.0133978795724885</v>
+        <v>-0.2029228915203793</v>
       </c>
       <c r="T2" t="n">
-        <v>-2.302445093265506</v>
+        <v>-3.923885890456292</v>
       </c>
       <c r="U2" t="n">
-        <v>-0.1217333909920973</v>
+        <v>-0.1069314005715102</v>
       </c>
       <c r="V2" t="n">
-        <v>-0.2034974350603995</v>
+        <v>-0.2450550893051696</v>
       </c>
       <c r="W2" t="n">
-        <v>-0.0652748201594214</v>
+        <v>-0.1746790447281685</v>
       </c>
       <c r="X2" t="n">
-        <v>-0.0889470042929378</v>
+        <v>-0.6591733937428546</v>
       </c>
       <c r="Y2" t="n">
-        <v>-0.030114001585058</v>
+        <v>-0.2845718212159317</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>02-22377202</t>
+          <t>02-22377333</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-2.213109886209192</v>
+        <v>-2.743705932690061</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0607637538432642</v>
+        <v>-0.2312986926860345</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.0139224732909524</v>
+        <v>-0.1723246136575217</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>-0.28510207521807</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.8378991726665036</v>
+        <v>-1.923022413006756</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.0280277107630275</v>
+        <v>-0.1731907618525601</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.0458648109761013</v>
+        <v>-0.2202452032826287</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.0846086633060856</v>
+        <v>-0.1477872634936202</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.0088385826553072</v>
+        <v>-0.1950650869396044</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.0312567391186001</v>
+        <v>-0.2021273158383511</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.0110873375064349</v>
+        <v>-0.1707091716913059</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.0531011461731492</v>
+        <v>-0.248443121635857</v>
       </c>
       <c r="N3" t="n">
-        <v>-1.89144994102389</v>
+        <v>-3.994690389837336</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.0584989297470962</v>
+        <v>-0.2313150841287662</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.0243127997239618</v>
+        <v>-0.2541147779691275</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.08621988816611249</v>
+        <v>-0.09351753234984</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.0523858229060097</v>
+        <v>-0.2241456265118556</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.1037873588659301</v>
+        <v>-0.2419646114533808</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.0105956812416946</v>
+        <v>-0.5467119291425644</v>
       </c>
       <c r="U3" t="n">
-        <v>-0.0154334637361122</v>
+        <v>-0.1556295336383683</v>
       </c>
       <c r="V3" t="n">
-        <v>-0.0529075053976638</v>
+        <v>-0.2652024934949402</v>
       </c>
       <c r="W3" t="n">
-        <v>-0.0236952423762299</v>
+        <v>-0.1269994073347251</v>
       </c>
       <c r="X3" t="n">
-        <v>-0.9206084642321344</v>
+        <v>-1.918749702830708</v>
       </c>
       <c r="Y3" t="n">
-        <v>-0.1098301738996068</v>
+        <v>-0.2757722619035998</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>03-21377053</t>
+          <t>03-21377348</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.0944580958714154</v>
+        <v>-0.3839672208490632</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0494246528697268</v>
+        <v>-0.3386142828359892</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.078549634351003</v>
+        <v>-0.1480089003759244</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.0090605806606804</v>
+        <v>-0.1712714320698662</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.480185538513142</v>
+        <v>-2.954008831978041</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.0196849059739982</v>
+        <v>-0.09563825351603911</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.0893882378604581</v>
+        <v>-0.2110657213173712</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>-0.2812376897188197</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.0419521730729267</v>
+        <v>-0.2672626366537691</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.0225329210877704</v>
+        <v>-0.2139183512767008</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.0515150275206332</v>
+        <v>-0.235022168149464</v>
       </c>
       <c r="M4" t="n">
-        <v>-2.502515104483944</v>
+        <v>-5.340621974511906</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.6434866652500002</v>
+        <v>-3.308397952575144</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.0438213292989482</v>
+        <v>-0.2179372333033001</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.0697493562487687</v>
+        <v>-0.1729342369512843</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>-0.1316056211524975</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.0482291835627392</v>
+        <v>-0.2129447435987096</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.036129960854603</v>
+        <v>-0.1544141553847059</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.0841969353991099</v>
+        <v>-0.2458336088193255</v>
       </c>
       <c r="U4" t="n">
-        <v>-0.05178762388808</v>
+        <v>-0.2481095744187489</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.2110356578635301</v>
+        <v>-0.2275002436082831</v>
       </c>
       <c r="W4" t="n">
-        <v>-0.0139224732909524</v>
+        <v>-0.2104344188571157</v>
       </c>
       <c r="X4" t="n">
-        <v>-1.271190658859351</v>
+        <v>-4.461682688658707</v>
       </c>
       <c r="Y4" t="n">
-        <v>-0.1086271838907662</v>
+        <v>-0.370447729633947</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>04-21377256</t>
+          <t>04-21379216</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.0082342722271718</v>
+        <v>-0.2801336117703973</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.6108936955302962</v>
+        <v>-4.412219721411679</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0196849059739982</v>
+        <v>-0.1173242435862268</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.0164623613185196</v>
+        <v>-0.2720232594416418</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.626083036965945</v>
+        <v>-2.458726118755425</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.0120315235820931</v>
+        <v>-0.2474950555523318</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.0196849059739982</v>
+        <v>-0.1645339432567648</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.0536950313191359</v>
+        <v>-0.2356849658429507</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.0131490025525661</v>
+        <v>-0.0743391154624015</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.0519054069160566</v>
+        <v>-0.2227943477600294</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.1095533232473706</v>
+        <v>-0.2185842403132718</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.4039782068813599</v>
+        <v>-4.371523998056158</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.6992559321225985</v>
+        <v>-1.616637425739022</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.0157788030630794</v>
+        <v>-0.2992202418308577</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.0147926278716369</v>
+        <v>-0.1151926151270294</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.0139224732909524</v>
+        <v>-0.2457885222571144</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.0257763973462078</v>
+        <v>-0.3152088018965961</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.0208322214997017</v>
+        <v>-0.1638814994059579</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.0144917608640782</v>
+        <v>-0.1993931959064149</v>
       </c>
       <c r="U5" t="n">
-        <v>-0.0269415906863181</v>
+        <v>-0.2506994912096305</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.0477173505086763</v>
+        <v>-0.1561895494354033</v>
       </c>
       <c r="W5" t="n">
-        <v>-0.0711913248480171</v>
+        <v>-0.07701644540036361</v>
       </c>
       <c r="X5" t="n">
-        <v>0</v>
+        <v>-0.4243496824035254</v>
       </c>
       <c r="Y5" t="n">
-        <v>-0.0173057840046677</v>
+        <v>-0.2279046901903983</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05-21377006</t>
+          <t>05-21377151</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>-0.2484480276055178</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.7607604412641606</v>
+        <v>-1.536190883186174</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.0473810427861689</v>
+        <v>-0.2830411857466908</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.0590716772256032</v>
+        <v>-0.1215123563331318</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.0519648616862995</v>
+        <v>-0.4811265136746071</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.0236288192723708</v>
+        <v>-0.3331961330361436</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.1000248493635591</v>
+        <v>-0.2236655875279546</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.0181898498240743</v>
+        <v>-0.1996065932691842</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.0251885386779911</v>
+        <v>-0.2653247219477335</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.0923933566879446</v>
+        <v>-0.2896324530467291</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.0212902592446309</v>
+        <v>-0.3285481423975049</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.651096404244202</v>
+        <v>-3.422156180654887</v>
       </c>
       <c r="N6" t="n">
-        <v>-1.502384000602138</v>
+        <v>-4.41175282316089</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.1549626261230512</v>
+        <v>-0.1752929132664228</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.1095533232473706</v>
+        <v>-0.1630746545433659</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.1080486720642838</v>
+        <v>-0.1238936809425077</v>
       </c>
       <c r="R6" t="n">
-        <v>-1.05862963226189</v>
+        <v>-5.396466262156039</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.0945613288318231</v>
+        <v>-0.2362924964942701</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.132129239810334</v>
+        <v>-0.1716760506962965</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.1192877511568803</v>
+        <v>-0.2509981392729802</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.0279610123164152</v>
+        <v>-0.1749250550920702</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.0591705114865478</v>
+        <v>-0.1533977087235725</v>
       </c>
       <c r="X6" t="n">
-        <v>-0.0193657265836114</v>
+        <v>-0.2847142758580021</v>
       </c>
       <c r="Y6" t="n">
-        <v>-0.0308669274722244</v>
+        <v>-0.1784712175444098</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06-21377242</t>
+          <t>06-21377076</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.0243362439233758</v>
+        <v>-0.214685384057911</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.5105480844030447</v>
+        <v>-2.534922772614459</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0304883465779281</v>
+        <v>-0.109562841959286</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0639248739853993</v>
+        <v>-0.2419646114533808</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.0617907834375667</v>
+        <v>-0.2557673177540793</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.050071401720172</v>
+        <v>-0.2151586029643116</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.9793202352437068</v>
+        <v>-3.430496820900363</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.0302260916077491</v>
+        <v>-0.307636516207925</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.0227635769429334</v>
+        <v>-0.1477137603716813</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.1488730069001543</v>
+        <v>-0.1526296310799954</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.0799554295648772</v>
+        <v>-0.2091210445432466</v>
       </c>
       <c r="M7" t="n">
-        <v>-1.647569275723863</v>
+        <v>-1.952797899744878</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.041214799294087</v>
+        <v>-0.3785795040441574</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.0788554174605461</v>
+        <v>-0.2418503251295176</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.0117033007012369</v>
+        <v>-0.1590307408575714</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.0658494452740787</v>
+        <v>-0.1517219663554407</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.3323130912313325</v>
+        <v>-1.737186125928117</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.0144917608640782</v>
+        <v>-0.1348706324541136</v>
       </c>
       <c r="T7" t="n">
-        <v>-0.0571591457953144</v>
+        <v>-0.2675506229209076</v>
       </c>
       <c r="U7" t="n">
-        <v>-0.0094561569473213</v>
+        <v>-0.3726848047872922</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.0343691362525433</v>
+        <v>-0.2737625238007136</v>
       </c>
       <c r="W7" t="n">
-        <v>-0.0473810427861689</v>
+        <v>-0.1612921715413143</v>
       </c>
       <c r="X7" t="n">
-        <v>-0.0110873375064349</v>
+        <v>-0.2720983580470456</v>
       </c>
       <c r="Y7" t="n">
-        <v>0</v>
+        <v>-0.3974678377151713</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>07-sy2308207</t>
+          <t>07-21377259</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.0574867005413692</v>
+        <v>-0.3021616251575142</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.283048405716696</v>
+        <v>-5.156007983930325</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0147926278716369</v>
+        <v>-0.3212445169996948</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>-0.1892508081048877</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.0312567391186001</v>
+        <v>-0.1657794421278333</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.0101361095251873</v>
+        <v>-0.2338731810287229</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.2448679663180328</v>
+        <v>-2.739365779378104</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.0298214781132568</v>
+        <v>-0.1610848102273771</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.0196849059739982</v>
+        <v>-0.1333517035875975</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.0269367950003466</v>
+        <v>-0.1537984706038911</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.06637302482504299</v>
+        <v>-0.1078333829889273</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.0842932467078935</v>
+        <v>-0.4198082638080514</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.0256883968861049</v>
+        <v>-0.2624503199345269</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.0228253799873337</v>
+        <v>-0.4264592219519091</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.0116356124380718</v>
+        <v>-0.1954853800924321</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.07973718980775819</v>
+        <v>-0.290615565751549</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.5476613656198444</v>
+        <v>-2.188637085641329</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.0628695285236435</v>
+        <v>-0.236173463957041</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.1033678813380925</v>
+        <v>-0.2973738545010541</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.2456729474035726</v>
+        <v>-0.2256741139071317</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.0596088115716333</v>
+        <v>-0.1183128313754552</v>
       </c>
       <c r="W8" t="n">
-        <v>-0.0132355091483067</v>
+        <v>-0.3060950246216638</v>
       </c>
       <c r="X8" t="n">
-        <v>-0.012282035351298</v>
+        <v>-0.2104518089247588</v>
       </c>
       <c r="Y8" t="n">
-        <v>-0.2719287675740032</v>
+        <v>-3.73685015463312</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>08-21377175</t>
+          <t>08-y2342116</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.1033678813380925</v>
+        <v>-0.2353430259020729</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.0538927927999941</v>
+        <v>-0.4688169239541084</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.0157788030630794</v>
+        <v>-0.1974376914893112</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0208322214997017</v>
+        <v>-0.2196301224567804</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.0320407377306989</v>
+        <v>-0.2116976460242264</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.07066643383325689</v>
+        <v>-0.2069244173611852</v>
       </c>
       <c r="H9" t="n">
-        <v>-1.138160510077234</v>
+        <v>-2.723919106389538</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.0858593183342581</v>
+        <v>-0.1930983123579015</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.07329841886802931</v>
+        <v>-0.2563624823978459</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.012677993505907</v>
+        <v>-0.1772671477586547</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0269333436023433</v>
+        <v>-0.2532354186633486</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0299579930441067</v>
+        <v>-0.2049168732267466</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.0144917608640782</v>
+        <v>-0.1899504096681144</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.549886635436612</v>
+        <v>-5.67202382709695</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.0181898498240743</v>
+        <v>-0.1544818361132032</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.01820631122663</v>
+        <v>-0.1723384398240619</v>
       </c>
       <c r="R9" t="n">
-        <v>-1.189197458077978</v>
+        <v>-6.271273246768422</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.0129156176885289</v>
+        <v>-0.0752908513137672</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.0453024228568881</v>
+        <v>-0.1476265364472245</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.0691284950552481</v>
+        <v>-0.2134729468770941</v>
       </c>
       <c r="V9" t="n">
-        <v>-0.0287151011625893</v>
+        <v>-0.2034029846997183</v>
       </c>
       <c r="W9" t="n">
-        <v>-0.0165060596714404</v>
+        <v>-0.2098142154835639</v>
       </c>
       <c r="X9" t="n">
-        <v>-0.0319395234075526</v>
+        <v>-0.1436950521962303</v>
       </c>
       <c r="Y9" t="n">
-        <v>-0.205642153662269</v>
+        <v>-3.438074829508952</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>09-21377163</t>
+          <t>09-21377174</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.0876488951101471</v>
+        <v>-0.2109353721769505</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.0249545032767572</v>
+        <v>-0.1861659257112728</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.0740497445469722</v>
+        <v>-0.2590136163970371</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.0491281414051923</v>
+        <v>-0.2045504967588473</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.0288313433086007</v>
+        <v>-0.1670974287035748</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.07460397522266</v>
+        <v>-0.1549008113966921</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.9259064983364182</v>
+        <v>-2.188469764444124</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.0181898498240743</v>
+        <v>-0.32361502490747</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.01820631122663</v>
+        <v>-0.280133580114955</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>-0.1188423607803558</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.4637751412564415</v>
+        <v>-4.830470339299909</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.0231812440597992</v>
+        <v>-0.225890804801812</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.0376838527799397</v>
+        <v>-0.2292195588899402</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.6220088931032466</v>
+        <v>-1.66039212046282</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.0319395234075526</v>
+        <v>-0.2821523268049887</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>-0.1691500980674463</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.0297682457159937</v>
+        <v>-0.5255200413875354</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.0228058003786208</v>
+        <v>-0.0981478582056927</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.0181898498240743</v>
+        <v>-0.1068721920982735</v>
       </c>
       <c r="U10" t="n">
-        <v>-0.0278280778031281</v>
+        <v>-0.3276154737210147</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.0326970487335397</v>
+        <v>-0.1527959243476426</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.0118341022973095</v>
+        <v>-0.2866058769622192</v>
       </c>
       <c r="X10" t="n">
-        <v>-0.0681900003404867</v>
+        <v>-0.3188060911883699</v>
       </c>
       <c r="Y10" t="n">
-        <v>-0.4858693994033511</v>
+        <v>-2.683482998196028</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10-sy2308220</t>
+          <t>10-21377335</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.0208322214997017</v>
+        <v>-0.193264320160048</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0111497204777061</v>
+        <v>-0.2055010364550178</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.0196849059739982</v>
+        <v>-0.230775972896508</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.0181898498240743</v>
+        <v>-0.071631070003578</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.552923681028325</v>
+        <v>-0.2267164485314156</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.0587235321918566</v>
+        <v>-0.2548373932806324</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.0628764623051488</v>
+        <v>-0.4858262811975548</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.0321287845175825</v>
+        <v>-0.0760996582204007</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.1217844515599227</v>
+        <v>-0.2151586029643116</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.0320984118763047</v>
+        <v>-0.19842134190315</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.5077779704048159</v>
+        <v>-3.191865965198373</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.08341521537643889</v>
+        <v>-0.1438020001443103</v>
       </c>
       <c r="N11" t="n">
-        <v>-0.0263887960608492</v>
+        <v>-0.1628504934511548</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.4441648862281129</v>
+        <v>-2.825591450027236</v>
       </c>
       <c r="P11" t="n">
-        <v>-0.0263325552412552</v>
+        <v>-0.1320788721617115</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.0157788030630794</v>
+        <v>-0.1785402658021609</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.0299579930441067</v>
+        <v>-0.3095960150794011</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.0423536292745815</v>
+        <v>-0.3423166493074787</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.0139224732909524</v>
+        <v>-0.1556001758968664</v>
       </c>
       <c r="U11" t="n">
-        <v>-1.198823938838565</v>
+        <v>-5.711066953564529</v>
       </c>
       <c r="V11" t="n">
-        <v>-0.0201179739054262</v>
+        <v>-0.08760709496789069</v>
       </c>
       <c r="W11" t="n">
-        <v>-0.0291648002015505</v>
+        <v>-0.2130877790380724</v>
       </c>
       <c r="X11" t="n">
-        <v>-0.0368050040189492</v>
+        <v>-0.1642965064899644</v>
       </c>
       <c r="Y11" t="n">
-        <v>-0.5334039906311405</v>
+        <v>-2.200792746963684</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11-22377339</t>
+          <t>11-21377187</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.1855100801392331</v>
+        <v>-0.1803324082311102</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.2664137920942788</v>
+        <v>-0.2574866747256574</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.0313546402877263</v>
+        <v>-0.4065365805919433</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.09617599534464739</v>
+        <v>-0.1813914029784039</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.1282027748875202</v>
+        <v>-0.1518377016375832</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.5409214064234986</v>
+        <v>-4.42116846819554</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.0864059335200688</v>
+        <v>-0.2877230315246539</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.0567439605423045</v>
+        <v>-0.1803206084892996</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.0347322258659417</v>
+        <v>-0.327130522471287</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.0604977969875368</v>
+        <v>-0.1408314748273205</v>
       </c>
       <c r="L12" t="n">
-        <v>-1.099541385453776</v>
+        <v>-3.357446822573279</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.0503507153564023</v>
+        <v>-0.2229586585271907</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.3438844826720373</v>
+        <v>-0.2312744474938372</v>
       </c>
       <c r="O12" t="n">
-        <v>-1.569048556982363</v>
+        <v>-4.993018518448976</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.0806420731457156</v>
+        <v>-0.0908148736679809</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.0567439605423045</v>
+        <v>-0.2354817621737281</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0124569497866416</v>
+        <v>-0.2166694592226334</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.1655882391224466</v>
+        <v>-0.2051829634457451</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.0618315130200671</v>
+        <v>-0.1114413122299586</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.9344951900981224</v>
+        <v>-4.403698243219495</v>
       </c>
       <c r="V12" t="n">
-        <v>-0.0181898498240743</v>
+        <v>-0.2435103024756243</v>
       </c>
       <c r="W12" t="n">
-        <v>-0.1632154503584075</v>
+        <v>-0.198540509477545</v>
       </c>
       <c r="X12" t="n">
-        <v>-0.0352560331310865</v>
+        <v>-0.159174868807218</v>
       </c>
       <c r="Y12" t="n">
-        <v>-0.0279014652463623</v>
+        <v>-0.3377886097371552</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>12-20377292</t>
+          <t>12-22377142</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.0432810810105213</v>
+        <v>-0.1076016644954203</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.0702010909905763</v>
+        <v>-0.2153668962249375</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.3234114257963367</v>
+        <v>-2.484128031789629</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.070700651642153</v>
+        <v>-0.1204766059498047</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.06846502481262499</v>
+        <v>-0.1540733544041139</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.4262538285970643</v>
+        <v>-3.172316361062457</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.0136300636215625</v>
+        <v>-0.2112294207461499</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.0157788030630794</v>
+        <v>-0.0811382791632622</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.0733914888961788</v>
+        <v>-0.2162882397415376</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.0756765711579882</v>
+        <v>-0.1379681915684926</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.7539953549530305</v>
+        <v>-5.042072906320223</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.1171852384384187</v>
+        <v>-0.2235927062995647</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.0796566574634459</v>
+        <v>-0.1683052831902896</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.0252980734943885</v>
+        <v>-0.4702400445773195</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.0456855855111058</v>
+        <v>-0.3269867954532419</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.100229981777951</v>
+        <v>-0.1363629971014983</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.0351079414042428</v>
+        <v>-0.2264571591635502</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.0474360647875313</v>
+        <v>-0.1796737114244229</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.0561428797550105</v>
+        <v>-0.1551984138292701</v>
       </c>
       <c r="U13" t="n">
-        <v>-0.6707232851281895</v>
+        <v>-1.769184562781304</v>
       </c>
       <c r="V13" t="n">
-        <v>-0.0240656967151563</v>
+        <v>-0.2622079269857636</v>
       </c>
       <c r="W13" t="n">
-        <v>-0.0542448800487531</v>
+        <v>-0.546470418940444</v>
       </c>
       <c r="X13" t="n">
-        <v>-0.0676658465312374</v>
+        <v>-0.1899752099129112</v>
       </c>
       <c r="Y13" t="n">
-        <v>-0.1136907659727978</v>
+        <v>-0.2393428333001473</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13-20377387</t>
+          <t>13-21377181</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.1412904796546329</v>
+        <v>-0.2178095149060589</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.0686029767391873</v>
+        <v>-0.246245337529937</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.4166181969575169</v>
+        <v>-1.272486857236578</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.0845095949834596</v>
+        <v>-0.0576419161217382</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.1666074927881969</v>
+        <v>-0.1794773778533306</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.2755107946289719</v>
+        <v>-2.074836878962162</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.100889712485216</v>
+        <v>-0.1612546357808549</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.0733565016221239</v>
+        <v>-0.2129818120772715</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.1303020760203825</v>
+        <v>-0.2508436562198721</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.0154578782550167</v>
+        <v>-0.2239695596897642</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.0605824743741203</v>
+        <v>-0.2562829093590534</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.0370838228671451</v>
+        <v>-0.09708000914863101</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.0181898498240743</v>
+        <v>-0.2180466620928895</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.1837644503230545</v>
+        <v>-0.2980926565199879</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.2197618390244012</v>
+        <v>-0.2242202439452038</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.1554103674189174</v>
+        <v>-0.1749792897924859</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.0217495049827802</v>
+        <v>-0.1660283543698687</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.1047064336597596</v>
+        <v>-0.3472554625241206</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.1126909648392684</v>
+        <v>-0.0759010331230701</v>
       </c>
       <c r="U14" t="n">
-        <v>-1.014387745128064</v>
+        <v>-5.171401074780791</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.1811489894249227</v>
+        <v>-0.197070403345395</v>
       </c>
       <c r="W14" t="n">
-        <v>-1.060658484193921</v>
+        <v>-3.950749336837884</v>
       </c>
       <c r="X14" t="n">
-        <v>-0.0541418561194191</v>
+        <v>-0.1258471192094757</v>
       </c>
       <c r="Y14" t="n">
-        <v>-0.0232772200392719</v>
+        <v>-0.1319297571996327</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>14-20377359</t>
+          <t>14-21377369</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.08918377167532469</v>
+        <v>-0.07235093037758041</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.0918079953402529</v>
+        <v>-0.1561730275907752</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.578547128522348</v>
+        <v>-0.5679749570429172</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.0618315130200671</v>
+        <v>-0.280889353493052</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.1194275963303975</v>
+        <v>-0.1134004989076708</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.7343641919813109</v>
+        <v>-4.538673356603685</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.0538850453553101</v>
+        <v>-0.1885287481336269</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.0812829090101909</v>
+        <v>-0.1063440939728545</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.1110781982375558</v>
+        <v>-0.3336206481075036</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.0641746017999302</v>
+        <v>-0.2288461296870272</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.09673811929628</v>
+        <v>-0.3258848195562305</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.0605370286275834</v>
+        <v>-0.1646791296329492</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.063754018271849</v>
+        <v>-0.260312701750531</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>-0.1497544855186837</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.0427448868198433</v>
+        <v>-0.2061440297367147</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.6236091498325921</v>
+        <v>-0.2597417764550783</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.2052175850565322</v>
+        <v>-0.2284341630094389</v>
       </c>
       <c r="S15" t="n">
-        <v>-0.151780311624314</v>
+        <v>-0.2009538032010009</v>
       </c>
       <c r="T15" t="n">
-        <v>-0.0319258392903513</v>
+        <v>-0.1027284665225282</v>
       </c>
       <c r="U15" t="n">
-        <v>-0.0822536817619189</v>
+        <v>-0.5081225409256231</v>
       </c>
       <c r="V15" t="n">
-        <v>-0.0588975298032352</v>
+        <v>-0.3597607091217497</v>
       </c>
       <c r="W15" t="n">
-        <v>-0.782103275833809</v>
+        <v>-4.154108410425945</v>
       </c>
       <c r="X15" t="n">
-        <v>0</v>
+        <v>-0.2428028577109389</v>
       </c>
       <c r="Y15" t="n">
-        <v>-0.1552971184244885</v>
+        <v>-0.176497898333153</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>15-BY2308108</t>
+          <t>15-22377053</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.093636113741973</v>
+        <v>-0.1285689406360023</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.0691487824891128</v>
+        <v>-0.2000565961959846</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.6711115594703665</v>
+        <v>-1.781652896272867</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.01681030014216</v>
+        <v>-0.1476852087547924</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.0313381432152879</v>
+        <v>-0.2096615284879376</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.0168011498323184</v>
+        <v>-0.3418535363896339</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.06859207654793339</v>
+        <v>-0.2213085524171982</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.0377275511328605</v>
+        <v>-0.1804987005112139</v>
       </c>
       <c r="J16" t="n">
-        <v>-1.13748015344017</v>
+        <v>-4.343799319416816</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.315912940903605</v>
+        <v>-0.2211556310459456</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.0226964917019065</v>
+        <v>-0.2082970539703443</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.06922949843926091</v>
+        <v>-0.2616862922519715</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.08879361617107109</v>
+        <v>-0.1612218994375699</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.09451258477546839</v>
+        <v>-0.2606167552054468</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.0142044408845447</v>
+        <v>-0.3309899025708954</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.127163300341613</v>
+        <v>-0.5944495327202137</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.1531191032174139</v>
+        <v>-0.1643626902048818</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.09895845191792541</v>
+        <v>-0.1001327639579463</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.0423536292745815</v>
+        <v>-0.3704155200341392</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.0566739580748324</v>
+        <v>-0.2184060232024099</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.0524825295418522</v>
+        <v>-0.2085840185217486</v>
       </c>
       <c r="W16" t="n">
-        <v>-0.48838757551357</v>
+        <v>-1.866141067854455</v>
       </c>
       <c r="X16" t="n">
-        <v>-0.0988742663843184</v>
+        <v>-0.1290407437420958</v>
       </c>
       <c r="Y16" t="n">
-        <v>-0.0756765711579882</v>
+        <v>-0.2755762248347267</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16-by2308145</t>
+          <t>16-22377084</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.0495669206170034</v>
+        <v>-0.0729861378894533</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.1283646842473093</v>
+        <v>-0.0642513780055862</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>-0.1974033115692772</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.2120671131677873</v>
+        <v>-0.0627350001303157</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.0254548438965711</v>
+        <v>-0.0375901776170379</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.0910983888597523</v>
+        <v>-0.1233031652701594</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.1148566011110692</v>
+        <v>-0.1026326443376219</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.42874156671004</v>
+        <v>-1.039297678776294</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.3732466043322739</v>
+        <v>-0.3482271813755371</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.07242470605953449</v>
+        <v>-0.1176557020998695</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.1112405615947098</v>
+        <v>-0.1010778314721693</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.0245967864460402</v>
+        <v>-0.0491474802475557</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>-0.1858700615815864</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.1090431565229192</v>
+        <v>-0.0638287182632163</v>
       </c>
       <c r="P17" t="n">
-        <v>-0.093576671867891</v>
+        <v>-0.0546949070036189</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.3369635827831941</v>
+        <v>-1.689354636139058</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.0588403434694541</v>
+        <v>-0.1494833974396997</v>
       </c>
       <c r="S17" t="n">
-        <v>0</v>
+        <v>-0.2609718867971906</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.1051629579351032</v>
+        <v>-0.0181673718727708</v>
       </c>
       <c r="U17" t="n">
-        <v>-0.0120315235820931</v>
+        <v>-0.0480142575308502</v>
       </c>
       <c r="V17" t="n">
-        <v>0</v>
+        <v>-0.0131183807487642</v>
       </c>
       <c r="W17" t="n">
-        <v>-2.197501765054252</v>
+        <v>-3.797787105973767</v>
       </c>
       <c r="X17" t="n">
-        <v>0</v>
+        <v>-0.0218246625140228</v>
       </c>
       <c r="Y17" t="n">
-        <v>-0.0608339443600199</v>
+        <v>-0.10816300496229</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>17-zy2308131</t>
+          <t>17-21377185</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0634697318254195</v>
+        <v>-0.0543852427855678</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>-0.0454563985630189</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>-0.0680668510030956</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>-0.043952410037332</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.0163798566255287</v>
+        <v>-0.024220883422897</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.0161347159141263</v>
+        <v>-0.0543598701418484</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.0161347159141263</v>
+        <v>-0.0146236570444427</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.2294936174247153</v>
+        <v>-0.2632258267999697</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.5500762406213893</v>
+        <v>-2.43573437012321</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>-0.0918744902465969</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.0281416721095123</v>
+        <v>-0.0615931708302025</v>
       </c>
       <c r="M18" t="n">
-        <v>-0.062868668454457</v>
+        <v>-0.105571587581616</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.2340088230499257</v>
+        <v>-0.0083144394000285</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.0147926278716369</v>
+        <v>-0.0134901865838135</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.0351183697101104</v>
+        <v>-0.159386823269042</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.1311265290935072</v>
+        <v>-1.406524874878081</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.0154334637361122</v>
+        <v>-0.1659645800574605</v>
       </c>
       <c r="S18" t="n">
-        <v>-0.4550120074195214</v>
+        <v>-0.8799257252212596</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.050071401720172</v>
+        <v>-0.0617028064637351</v>
       </c>
       <c r="U18" t="n">
-        <v>-0.0320407377306989</v>
+        <v>-0.1133359768083256</v>
       </c>
       <c r="V18" t="n">
-        <v>-0.0149022028929083</v>
+        <v>-0.2675459209444684</v>
       </c>
       <c r="W18" t="n">
-        <v>-0.0114543329689279</v>
+        <v>-0.1209976604400142</v>
       </c>
       <c r="X18" t="n">
-        <v>-0.0131490025525661</v>
+        <v>-0.0729861378894533</v>
       </c>
       <c r="Y18" t="n">
-        <v>-0.0329247226370393</v>
+        <v>-0.1296520143040819</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18-BY2308106</t>
+          <t>18-21377184</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.0129209851672615</v>
+        <v>-0.07353264250909761</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.0104336498330829</v>
+        <v>-0.1331209290434096</v>
       </c>
       <c r="D19" t="n">
+        <v>-0.0136393043426618</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-0.0548482323099486</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-0.0729861378894533</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-0.0394470076576985</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-0.07931905318388589</v>
+      </c>
+      <c r="I19" t="n">
+        <v>-1.807045986946725</v>
+      </c>
+      <c r="J19" t="n">
+        <v>-4.038213278115351</v>
+      </c>
+      <c r="K19" t="n">
+        <v>-0.0131183807487642</v>
+      </c>
+      <c r="L19" t="n">
+        <v>-0.0493237278911885</v>
+      </c>
+      <c r="M19" t="n">
+        <v>-0.0081740279265479</v>
+      </c>
+      <c r="N19" t="n">
+        <v>-0.0136316028721126</v>
+      </c>
+      <c r="O19" t="n">
+        <v>-0.0859279684534608</v>
+      </c>
+      <c r="P19" t="n">
+        <v>-0.0962070750731633</v>
+      </c>
+      <c r="Q19" t="n">
         <v>0</v>
       </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
-        <v>-0.0100589869527131</v>
-      </c>
-      <c r="G19" t="n">
-        <v>-0.0488873412109763</v>
-      </c>
-      <c r="H19" t="n">
-        <v>-0.1188885911229006</v>
-      </c>
-      <c r="I19" t="n">
-        <v>-0.1716600815840169</v>
-      </c>
-      <c r="J19" t="n">
-        <v>-1.129395168750167</v>
-      </c>
-      <c r="K19" t="n">
-        <v>-0.012677993505907</v>
-      </c>
-      <c r="L19" t="n">
-        <v>-0.0567439605423045</v>
-      </c>
-      <c r="M19" t="n">
-        <v>-0.1379789542105799</v>
-      </c>
-      <c r="N19" t="n">
-        <v>-0.0965642061927237</v>
-      </c>
-      <c r="O19" t="n">
-        <v>-0.0747283047781848</v>
-      </c>
-      <c r="P19" t="n">
-        <v>-0.0165620124160894</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>-0.0284550889279535</v>
-      </c>
       <c r="R19" t="n">
-        <v>-0.0229969618069706</v>
+        <v>-0.015603968680109</v>
       </c>
       <c r="S19" t="n">
-        <v>-0.374973932543614</v>
+        <v>-0.1504197208455711</v>
       </c>
       <c r="T19" t="n">
-        <v>-0.1086271838907662</v>
+        <v>-0.2277303991641657</v>
       </c>
       <c r="U19" t="n">
-        <v>-0.0220161277792512</v>
+        <v>-0.0691509335821122</v>
       </c>
       <c r="V19" t="n">
-        <v>-0.8867028436080464</v>
+        <v>-0.7525815028533481</v>
       </c>
       <c r="W19" t="n">
-        <v>-0.0551918297187903</v>
+        <v>-0.1468257572203463</v>
       </c>
       <c r="X19" t="n">
-        <v>-0.0239855715405192</v>
+        <v>-0.0146236570444427</v>
       </c>
       <c r="Y19" t="n">
-        <v>-0.0161347159141263</v>
+        <v>-0.0419620790224544</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19-BY2308111</t>
+          <t>19-y2314202</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.008335734207826</v>
+        <v>-0.2275302115323297</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.0157911883088118</v>
+        <v>-0.0375901776170379</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.0211991295104597</v>
+        <v>-0.0172760617478971</v>
       </c>
       <c r="E20" t="n">
+        <v>-0.0372137409685575</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-0.0122087968291504</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-0.0630783570010401</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-0.06806267173370489</v>
+      </c>
+      <c r="I20" t="n">
+        <v>-0.9231572800798428</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-0.4900887681671759</v>
+      </c>
+      <c r="K20" t="n">
+        <v>-0.3307744300033213</v>
+      </c>
+      <c r="L20" t="n">
+        <v>-0.143962832007875</v>
+      </c>
+      <c r="M20" t="n">
         <v>0</v>
       </c>
-      <c r="F20" t="n">
-        <v>-0.0316249920302178</v>
-      </c>
-      <c r="G20" t="n">
-        <v>-0.0186601497093808</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" t="n">
-        <v>-0.9513869652254968</v>
-      </c>
-      <c r="J20" t="n">
-        <v>-0.0444009499651964</v>
-      </c>
-      <c r="K20" t="n">
-        <v>-0.0165620124160894</v>
-      </c>
-      <c r="L20" t="n">
-        <v>-0.0447837388339222</v>
-      </c>
-      <c r="M20" t="n">
-        <v>-0.0596153981806467</v>
-      </c>
       <c r="N20" t="n">
-        <v>-0.0629764926482036</v>
+        <v>-0.0250847554930501</v>
       </c>
       <c r="O20" t="n">
-        <v>-0.0205914327449712</v>
+        <v>-0.025698983412964</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.320567199541786</v>
+        <v>-2.142245416871551</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.0142044408845447</v>
+        <v>-0.07824851899071179</v>
       </c>
       <c r="R20" t="n">
-        <v>-0.034093613445493</v>
+        <v>-0.1586514090997625</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.4615322041122023</v>
+        <v>-2.158268724452879</v>
       </c>
       <c r="T20" t="n">
-        <v>-0.02311164333899</v>
+        <v>-0.0666879462503502</v>
       </c>
       <c r="U20" t="n">
-        <v>-0.0681900003404867</v>
+        <v>-0.0551217338468724</v>
       </c>
       <c r="V20" t="n">
-        <v>-0.4068271136400047</v>
+        <v>-0.1459579535383476</v>
       </c>
       <c r="W20" t="n">
-        <v>0</v>
+        <v>-0.0476701689273228</v>
       </c>
       <c r="X20" t="n">
-        <v>-0.0218209208903655</v>
+        <v>-0.0480142575308502</v>
       </c>
       <c r="Y20" t="n">
-        <v>-0.1465545340713837</v>
+        <v>-0.0681717986316189</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20-ZY2207207</t>
+          <t>20-21377171</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.1085747777069844</v>
+        <v>-0.09151184163261659</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.1758007490348407</v>
+        <v>-0.0218246625140228</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.0531125781676869</v>
+        <v>-0.09591529945113531</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.0254071466052445</v>
+        <v>-0.1127543549973024</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.1899772747548592</v>
+        <v>-0.0480142575308502</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.3456632938120264</v>
+        <v>-0.0123612742890483</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.0239440588929457</v>
+        <v>-0.1331209290434096</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.041214799294087</v>
+        <v>-0.513802834155181</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.0543170117797391</v>
+        <v>-0.1574287113531201</v>
       </c>
       <c r="K21" t="n">
-        <v>-2.924277933598533</v>
+        <v>-1.082718588860935</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.0515153532376931</v>
+        <v>-0.1381096606779834</v>
       </c>
       <c r="M21" t="n">
-        <v>-0.079476516608433</v>
+        <v>-0.0250847554930501</v>
       </c>
       <c r="N21" t="n">
-        <v>-0.0551876822212335</v>
+        <v>-0.0122087968291504</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.0580573118164988</v>
+        <v>-0.1409057427528593</v>
       </c>
       <c r="P21" t="n">
-        <v>-0.7123237451592995</v>
+        <v>-0.8392580145057238</v>
       </c>
       <c r="Q21" t="n">
-        <v>-0.0235523415247586</v>
+        <v>-0.0307466568194297</v>
       </c>
       <c r="R21" t="n">
-        <v>-0.1103136948413541</v>
+        <v>-0.0332577576001142</v>
       </c>
       <c r="S21" t="n">
-        <v>-3.683940676188443</v>
+        <v>-4.207166645308037</v>
       </c>
       <c r="T21" t="n">
-        <v>-0.0810368230422904</v>
+        <v>-0.043198373210153</v>
       </c>
       <c r="U21" t="n">
-        <v>-0.1105551911246322</v>
+        <v>-0.1018631925016184</v>
       </c>
       <c r="V21" t="n">
-        <v>-1.630538138230026</v>
+        <v>-3.106237042606018</v>
       </c>
       <c r="W21" t="n">
-        <v>-0.0114213963777764</v>
+        <v>-0.0364126224532601</v>
       </c>
       <c r="X21" t="n">
-        <v>-0.0434152823324271</v>
+        <v>-0.1719925640976487</v>
       </c>
       <c r="Y21" t="n">
-        <v>-0.06558964001289309</v>
+        <v>-0.0699465656319402</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>21-by2308134</t>
+          <t>21-22377260</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.091473429738958</v>
+        <v>-0.1004381720985894</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.1027925673999881</v>
+        <v>-0.0676234416989117</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.0112660653870387</v>
+        <v>-0.09496927365797229</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.2723260033961938</v>
+        <v>-2.268575081899342</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.0362423226427218</v>
+        <v>-0.3094280772863711</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.0147926278716369</v>
+        <v>-0.1505918140279838</v>
       </c>
       <c r="H22" t="n">
+        <v>-0.009612027666233199</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-0.0993534168015346</v>
+      </c>
+      <c r="J22" t="n">
+        <v>-0.0237488307235518</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-0.1393548494823369</v>
+      </c>
+      <c r="L22" t="n">
+        <v>-0.0907307795464451</v>
+      </c>
+      <c r="M22" t="n">
+        <v>-0.0122087968291504</v>
+      </c>
+      <c r="N22" t="n">
+        <v>-0.0480142575308502</v>
+      </c>
+      <c r="O22" t="n">
+        <v>-0.0411197669291312</v>
+      </c>
+      <c r="P22" t="n">
+        <v>-1.889023682758824</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>-0.0195021175613825</v>
+      </c>
+      <c r="R22" t="n">
         <v>0</v>
       </c>
-      <c r="I22" t="n">
-        <v>-0.07273226298889281</v>
-      </c>
-      <c r="J22" t="n">
-        <v>-0.029913980807088</v>
-      </c>
-      <c r="K22" t="n">
-        <v>-0.4462051025084109</v>
-      </c>
-      <c r="L22" t="n">
-        <v>-0.1953968483364369</v>
-      </c>
-      <c r="M22" t="n">
-        <v>-0.1819520061831851</v>
-      </c>
-      <c r="N22" t="n">
-        <v>-0.1941817770148814</v>
-      </c>
-      <c r="O22" t="n">
-        <v>-0.1318194841010211</v>
-      </c>
-      <c r="P22" t="n">
-        <v>-0.1492267295182717</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>-0.0147926278716369</v>
-      </c>
-      <c r="R22" t="n">
-        <v>-0.0196849059739982</v>
-      </c>
       <c r="S22" t="n">
-        <v>-0.012462461711326</v>
+        <v>-0.2314334588190509</v>
       </c>
       <c r="T22" t="n">
-        <v>-0.0619309074803184</v>
+        <v>-0.1814803582370318</v>
       </c>
       <c r="U22" t="n">
-        <v>-0.0268847783063388</v>
+        <v>-0.111127855858545</v>
       </c>
       <c r="V22" t="n">
-        <v>-1.08097096153312</v>
+        <v>-1.814530814644098</v>
       </c>
       <c r="W22" t="n">
-        <v>-0.010955332324737</v>
+        <v>-0.0831776669136244</v>
       </c>
       <c r="X22" t="n">
-        <v>-0.110854452155594</v>
+        <v>-0.05541305462346</v>
       </c>
       <c r="Y22" t="n">
-        <v>-0.0154334637361122</v>
+        <v>-0.1126500031970772</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>22-22377318</t>
+          <t>22-21377225</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.1091977553126136</v>
+        <v>-0.171032165166083</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.014568926789872</v>
+        <v>-0.0133111406291542</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>-0.1618187911816529</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.3270180756684532</v>
+        <v>-0.3914012838151508</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.06737718572483969</v>
+        <v>-0.0828667836724135</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.0509570410535709</v>
+        <v>-0.0771081904998978</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.0116356124380718</v>
+        <v>-0.0685917964726432</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.0088951984843447</v>
+        <v>-0.0231737248825915</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.0283280919014917</v>
+        <v>-0.1003646195824334</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.8655630201335522</v>
+        <v>-4.173636614636651</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.0144917608640782</v>
+        <v>-0.0654586204090979</v>
       </c>
       <c r="M23" t="n">
-        <v>-0.1192877511568803</v>
+        <v>-0.0634981296955543</v>
       </c>
       <c r="N23" t="n">
-        <v>-0.0101361095251873</v>
+        <v>-0.233338097571984</v>
       </c>
       <c r="O23" t="n">
-        <v>0</v>
+        <v>-0.102444394261928</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.7355279440920617</v>
+        <v>-2.582098216035577</v>
       </c>
       <c r="Q23" t="n">
-        <v>-0.06541591164857451</v>
+        <v>-0.06696386840528851</v>
       </c>
       <c r="R23" t="n">
-        <v>-0.0585237780869179</v>
+        <v>-0.0729861378894533</v>
       </c>
       <c r="S23" t="n">
-        <v>-0.060577861538779</v>
+        <v>-0.1158310882059577</v>
       </c>
       <c r="T23" t="n">
-        <v>-1.333131479963416</v>
+        <v>-1.177079697899624</v>
       </c>
       <c r="U23" t="n">
-        <v>-0.0419521730729267</v>
+        <v>-0.084419927781586</v>
       </c>
       <c r="V23" t="n">
-        <v>-0.0116356124380718</v>
+        <v>-0.4163852478220526</v>
       </c>
       <c r="W23" t="n">
-        <v>-0.0881454808064297</v>
+        <v>-0.010577701143399</v>
       </c>
       <c r="X23" t="n">
-        <v>-0.0308669274722244</v>
+        <v>-0.08015095397249999</v>
       </c>
       <c r="Y23" t="n">
-        <v>0</v>
+        <v>-0.0352946910621513</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>23-21377298</t>
+          <t>23-22377206</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-1.333131479963416</v>
+        <v>-1.72769428924706</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.0461277150515245</v>
+        <v>-0.0620649059727352</v>
       </c>
       <c r="D24" t="n">
+        <v>-0.0514054603332652</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-2.079617554981024</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-0.0446301940003428</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-0.1234065801050809</v>
+      </c>
+      <c r="H24" t="n">
+        <v>-0.0729861378894533</v>
+      </c>
+      <c r="I24" t="n">
+        <v>-0.0154923891460928</v>
+      </c>
+      <c r="J24" t="n">
+        <v>-0.0634935948971205</v>
+      </c>
+      <c r="K24" t="n">
+        <v>-4.355271439518796</v>
+      </c>
+      <c r="L24" t="n">
+        <v>-0.0497416226712213</v>
+      </c>
+      <c r="M24" t="n">
+        <v>-0.2357404912913877</v>
+      </c>
+      <c r="N24" t="n">
+        <v>-0.09776144680367101</v>
+      </c>
+      <c r="O24" t="n">
+        <v>-0.07561117709421949</v>
+      </c>
+      <c r="P24" t="n">
+        <v>-0.3519553815110137</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>-0.0310483577004803</v>
+      </c>
+      <c r="R24" t="n">
+        <v>-0.0173025483714986</v>
+      </c>
+      <c r="S24" t="n">
+        <v>-0.0521524612309892</v>
+      </c>
+      <c r="T24" t="n">
+        <v>-1.119504490722905</v>
+      </c>
+      <c r="U24" t="n">
+        <v>-0.0459005423126708</v>
+      </c>
+      <c r="V24" t="n">
+        <v>-0.0544871052800991</v>
+      </c>
+      <c r="W24" t="n">
+        <v>-0.1980023124320684</v>
+      </c>
+      <c r="X24" t="n">
+        <v>-0.1801726160423861</v>
+      </c>
+      <c r="Y24" t="n">
         <v>0</v>
-      </c>
-      <c r="E24" t="n">
-        <v>-0.0373770262710385</v>
-      </c>
-      <c r="F24" t="n">
-        <v>-0.0797719185650311</v>
-      </c>
-      <c r="G24" t="n">
-        <v>-0.0861991693163834</v>
-      </c>
-      <c r="H24" t="n">
-        <v>-0.0618315130200671</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" t="n">
-        <v>-0.0147926278716369</v>
-      </c>
-      <c r="K24" t="n">
-        <v>-0.5988552208512871</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" t="n">
-        <v>-0.0498277991465665</v>
-      </c>
-      <c r="N24" t="n">
-        <v>-0.173784532713498</v>
-      </c>
-      <c r="O24" t="n">
-        <v>-0.0142113722952238</v>
-      </c>
-      <c r="P24" t="n">
-        <v>-0.0136624610563166</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" t="n">
-        <v>-0.0132355091483067</v>
-      </c>
-      <c r="S24" t="n">
-        <v>-0.0124569497866416</v>
-      </c>
-      <c r="T24" t="n">
-        <v>-0.4958150745364212</v>
-      </c>
-      <c r="U24" t="n">
-        <v>0</v>
-      </c>
-      <c r="V24" t="n">
-        <v>-0.0452634205987894</v>
-      </c>
-      <c r="W24" t="n">
-        <v>-0.0295852557432739</v>
-      </c>
-      <c r="X24" t="n">
-        <v>-0.0334096077725519</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>-0.0658494452740787</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>24-BY2308103</t>
+          <t>24-21377003</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.0799753640501968</v>
+        <v>-0.2380345147801695</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.0157788030630794</v>
+        <v>-0.1937329470938965</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.0591705114865478</v>
+        <v>-0.0277326272997106</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.2456121069063842</v>
+        <v>-1.544216174087171</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.0862643122217884</v>
+        <v>-0.157743528434103</v>
       </c>
       <c r="G25" t="n">
+        <v>-0.0725457192698839</v>
+      </c>
+      <c r="H25" t="n">
+        <v>-0.0146236570444427</v>
+      </c>
+      <c r="I25" t="n">
+        <v>-0.0466954315332916</v>
+      </c>
+      <c r="J25" t="n">
+        <v>-0.0123612742890483</v>
+      </c>
+      <c r="K25" t="n">
+        <v>-0.2138663155791179</v>
+      </c>
+      <c r="L25" t="n">
+        <v>-0.0309507290852711</v>
+      </c>
+      <c r="M25" t="n">
+        <v>-0.0952923431104913</v>
+      </c>
+      <c r="N25" t="n">
+        <v>-0.1652841486568196</v>
+      </c>
+      <c r="O25" t="n">
+        <v>-0.0235815078744923</v>
+      </c>
+      <c r="P25" t="n">
+        <v>-0.0883028513674125</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>-0.0315243335192709</v>
+      </c>
+      <c r="R25" t="n">
+        <v>-0.0599623859011907</v>
+      </c>
+      <c r="S25" t="n">
         <v>0</v>
       </c>
-      <c r="H25" t="n">
-        <v>-0.0697481218823012</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" t="n">
-        <v>-0.0658494452740787</v>
-      </c>
-      <c r="N25" t="n">
-        <v>0</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0</v>
-      </c>
-      <c r="P25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>0</v>
-      </c>
-      <c r="R25" t="n">
-        <v>0</v>
-      </c>
-      <c r="S25" t="n">
-        <v>-0.0186169799009149</v>
-      </c>
       <c r="T25" t="n">
-        <v>-0.2555245055349435</v>
+        <v>-2.340303873535126</v>
       </c>
       <c r="U25" t="n">
-        <v>0</v>
+        <v>-0.1070807816924472</v>
       </c>
       <c r="V25" t="n">
-        <v>0</v>
+        <v>-0.0481304333656822</v>
       </c>
       <c r="W25" t="n">
-        <v>-0.008746945176272201</v>
+        <v>-0.08430389065131</v>
       </c>
       <c r="X25" t="n">
-        <v>-0.409553032972941</v>
+        <v>-0.0196464588920178</v>
       </c>
       <c r="Y25" t="n">
-        <v>0</v>
+        <v>-0.127801281781441</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>25-SY2308310</t>
+          <t>25-22377028</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.3820056632868641</v>
+        <v>-2.305195091038109</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.0835009559943307</v>
+        <v>-0.2032887453419134</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.0691487824891128</v>
+        <v>-0.0458603050799701</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.0105956812416946</v>
+        <v>-0.0840641877183643</v>
       </c>
       <c r="F26" t="n">
-        <v>-1.611955974729059</v>
+        <v>-1.082718588860935</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.0516839406690462</v>
+        <v>-0.1042385072334024</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.2032501195409751</v>
+        <v>-0.0649789088058782</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.0609203429231614</v>
+        <v>-0.0685271402527769</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.1532655304065864</v>
+        <v>-0.1298498675652971</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.0496556947771395</v>
+        <v>-0.0827756147675396</v>
       </c>
       <c r="L26" t="n">
-        <v>-0.0588428884097021</v>
+        <v>-0.0218246625140228</v>
       </c>
       <c r="M26" t="n">
-        <v>-0.0248440605671657</v>
+        <v>-0.0393353862438397</v>
       </c>
       <c r="N26" t="n">
-        <v>-0.1303259602719318</v>
+        <v>-0.1142804140783293</v>
       </c>
       <c r="O26" t="n">
-        <v>-0.0508243551294979</v>
+        <v>-0.0729861378894533</v>
       </c>
       <c r="P26" t="n">
-        <v>-0.0239475213142918</v>
+        <v>-0.0551909693691993</v>
       </c>
       <c r="Q26" t="n">
-        <v>-0.0208322214997017</v>
+        <v>-0.1454603704858578</v>
       </c>
       <c r="R26" t="n">
-        <v>-0.0189127682554417</v>
+        <v>-0.4025218845419508</v>
       </c>
       <c r="S26" t="n">
-        <v>-0.1042214851054204</v>
+        <v>-0.0600677459708729</v>
       </c>
       <c r="T26" t="n">
-        <v>-2.069732744920577</v>
+        <v>-4.468102490361343</v>
       </c>
       <c r="U26" t="n">
-        <v>-0.0444614856496287</v>
+        <v>-0.0103036998235217</v>
       </c>
       <c r="V26" t="n">
-        <v>-0.0613739327683047</v>
+        <v>-0.0256350914030362</v>
       </c>
       <c r="W26" t="n">
-        <v>-0.0452634205987894</v>
+        <v>-0.0907307795464451</v>
       </c>
       <c r="X26" t="n">
-        <v>-0.1587441984285826</v>
+        <v>-0.2380345147801695</v>
       </c>
       <c r="Y26" t="n">
-        <v>-0.1194148638925827</v>
+        <v>-0.0146236570444427</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>26-22374085</t>
+          <t>26-22377005</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.5638456084114355</v>
+        <v>-2.72834248656879</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.0943915620039818</v>
+        <v>-0.1390573847549586</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>-0.041214799294087</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.1136907659727978</v>
+        <v>-0.1535908157376243</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.7418632944325851</v>
+        <v>-0.1392733816784831</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>-0.039086349301971</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.0646563640114374</v>
+        <v>-0.2173538409009886</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>-0.1026326443376219</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.012677993505907</v>
+        <v>-0.07100461378385731</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>-0.08643193779032091</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.0542865962527375</v>
+        <v>-0.1509203646002473</v>
       </c>
       <c r="M27" t="n">
-        <v>-0.1874676416381784</v>
+        <v>-0.1424449933431422</v>
       </c>
       <c r="N27" t="n">
-        <v>-0.6302973661275602</v>
+        <v>-1.091876766516151</v>
       </c>
       <c r="O27" t="n">
-        <v>-0.0551876822212335</v>
+        <v>-0.0460365535593278</v>
       </c>
       <c r="P27" t="n">
-        <v>-0.1210103693559473</v>
+        <v>-0.1106943722579109</v>
       </c>
       <c r="Q27" t="n">
-        <v>0</v>
+        <v>-0.0671875195376252</v>
       </c>
       <c r="R27" t="n">
-        <v>-0.0097147470045098</v>
+        <v>-0.0235714196021597</v>
       </c>
       <c r="S27" t="n">
-        <v>-0.1035780844733554</v>
+        <v>-0.01140216158775</v>
       </c>
       <c r="T27" t="n">
-        <v>0</v>
+        <v>-0.5067100504760045</v>
       </c>
       <c r="U27" t="n">
-        <v>-0.0280154690636006</v>
+        <v>-0.0154034254676493</v>
       </c>
       <c r="V27" t="n">
-        <v>-0.0138796670363645</v>
+        <v>-0.0471655612485393</v>
       </c>
       <c r="W27" t="n">
-        <v>0</v>
+        <v>-0.06422521002950719</v>
       </c>
       <c r="X27" t="n">
-        <v>-0.5460112592321776</v>
+        <v>-1.452260047340474</v>
       </c>
       <c r="Y27" t="n">
-        <v>0</v>
+        <v>-0.1190172573900847</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>27-22377099</t>
+          <t>27-21377255</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.041214799294087</v>
+        <v>-0.4408149919630556</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.08227067917089601</v>
+        <v>-0.1264023178601152</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.0294495571743168</v>
+        <v>-0.0267616871750869</v>
       </c>
       <c r="E28" t="n">
+        <v>-0.0436493250280456</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-1.621543836379059</v>
+      </c>
+      <c r="G28" t="n">
         <v>0</v>
       </c>
-      <c r="F28" t="n">
-        <v>-0.9514639219486996</v>
-      </c>
-      <c r="G28" t="n">
-        <v>-0.06529254391804119</v>
-      </c>
       <c r="H28" t="n">
-        <v>-0.1440214262216679</v>
+        <v>-0.0150399962306944</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.0468132028049476</v>
+        <v>-0.08430389065131</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.0116356124380718</v>
+        <v>-0.1693405082548202</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.112083966031593</v>
+        <v>-0.0272632057442253</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.1624111566814284</v>
+        <v>-0.0122087968291504</v>
       </c>
       <c r="M28" t="n">
-        <v>-2.065215572735576</v>
+        <v>-1.079372440129247</v>
       </c>
       <c r="N28" t="n">
-        <v>-0.2994889534750644</v>
+        <v>-0.1393548494823369</v>
       </c>
       <c r="O28" t="n">
-        <v>-0.1037873588659301</v>
+        <v>-0.0661781921644469</v>
       </c>
       <c r="P28" t="n">
-        <v>-0.0568004683676974</v>
+        <v>-0.0977772996135487</v>
       </c>
       <c r="Q28" t="n">
-        <v>-0.0120315235820931</v>
+        <v>-0.0629161595469938</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.0535877855109986</v>
+        <v>-0.0120270496173743</v>
       </c>
       <c r="S28" t="n">
-        <v>-0.1111785164133435</v>
+        <v>-0.1018631925016184</v>
       </c>
       <c r="T28" t="n">
-        <v>-0.0118341022973095</v>
+        <v>-0.0839712415834768</v>
       </c>
       <c r="U28" t="n">
-        <v>-0.0620538551357563</v>
+        <v>-0.1536550271356913</v>
       </c>
       <c r="V28" t="n">
-        <v>-0.4870278578939602</v>
+        <v>-0.0551217338468724</v>
       </c>
       <c r="W28" t="n">
-        <v>-0.012677993505907</v>
+        <v>-0.1556347611144545</v>
       </c>
       <c r="X28" t="n">
-        <v>-1.279503140385109</v>
+        <v>-3.959873550855171</v>
       </c>
       <c r="Y28" t="n">
-        <v>-0.0098859822631087</v>
+        <v>-0.2293827683493564</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>28-21377086</t>
+          <t>28-21081004</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.060577861538779</v>
+        <v>-0.1574287113531201</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.9679373541357872</v>
+        <v>-0.8202402318835409</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.0264282403097088</v>
+        <v>-0.0140328289765179</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.1270509570804752</v>
+        <v>-0.0172760617478971</v>
       </c>
       <c r="F29" t="n">
-        <v>-1.50511230740251</v>
+        <v>-2.738080636343843</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.0271436166565917</v>
+        <v>-0.0231702025045883</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.0831552292787464</v>
+        <v>-0.1265131143082821</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.0299252246001904</v>
+        <v>-0.0120270496173743</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.0558832608484062</v>
+        <v>-0.0395458254832459</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.0238765457544249</v>
+        <v>-0.1048915827464192</v>
       </c>
       <c r="L29" t="n">
-        <v>-0.0129209851672615</v>
+        <v>-0.0634981296955543</v>
       </c>
       <c r="M29" t="n">
-        <v>-0.3105388856362268</v>
+        <v>-0.4146766049893982</v>
       </c>
       <c r="N29" t="n">
-        <v>-0.5077226813542782</v>
+        <v>-3.50314382228441</v>
       </c>
       <c r="O29" t="n">
-        <v>-0.0142044408845447</v>
+        <v>-0.182771585738287</v>
       </c>
       <c r="P29" t="n">
-        <v>-0.0621175905021291</v>
+        <v>-0.0148372586630699</v>
       </c>
       <c r="Q29" t="n">
-        <v>-0.0165060596714404</v>
+        <v>-0.0313273470952844</v>
       </c>
       <c r="R29" t="n">
-        <v>-0.0269956622491723</v>
+        <v>-0.1143256865783743</v>
       </c>
       <c r="S29" t="n">
-        <v>-0.0602840597962599</v>
+        <v>-0.07100461378385731</v>
       </c>
       <c r="T29" t="n">
-        <v>0</v>
+        <v>-0.0481304333656822</v>
       </c>
       <c r="U29" t="n">
-        <v>-0.0197235038288492</v>
+        <v>-0.0133111406291542</v>
       </c>
       <c r="V29" t="n">
-        <v>-0.1476934587670887</v>
+        <v>-0.1578906256090044</v>
       </c>
       <c r="W29" t="n">
-        <v>-0.0329496768851888</v>
+        <v>-0.0144214866705564</v>
       </c>
       <c r="X29" t="n">
-        <v>-0.06735749237545249</v>
+        <v>-0.3067696753414278</v>
       </c>
       <c r="Y29" t="n">
-        <v>-0.0658494452740787</v>
+        <v>-0.0634381702097491</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>29-21377061</t>
+          <t>29-21377119</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.0124569497866416</v>
+        <v>-0.046751262093854</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.1828363532836481</v>
+        <v>-1.203968552455763</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.0208322214997017</v>
+        <v>-0.0285544260144044</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.0139224732909524</v>
+        <v>-0.043202059348191</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.0524735229950568</v>
+        <v>-0.2138663155791179</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.0334487630247837</v>
+        <v>-0.1291296691264669</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.1235221398984797</v>
+        <v>-0.131308586367063</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>-0.0471149701651106</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>-0.1934529714369116</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.0165060596714404</v>
+        <v>-0.0264119227309333</v>
       </c>
       <c r="L30" t="n">
-        <v>0</v>
+        <v>-0.1666416419370404</v>
       </c>
       <c r="M30" t="n">
-        <v>-0.3164713061180497</v>
+        <v>-2.087997455893972</v>
       </c>
       <c r="N30" t="n">
-        <v>-1.039494480267285</v>
+        <v>-3.789617225568161</v>
       </c>
       <c r="O30" t="n">
-        <v>-0.0116356124380718</v>
+        <v>-0.1011820602646807</v>
       </c>
       <c r="P30" t="n">
-        <v>0</v>
+        <v>-0.1035256270908617</v>
       </c>
       <c r="Q30" t="n">
-        <v>0</v>
+        <v>-0.0196495057373654</v>
       </c>
       <c r="R30" t="n">
-        <v>-0.5388593487325001</v>
+        <v>-1.030393455522352</v>
       </c>
       <c r="S30" t="n">
-        <v>-0.0591705114865478</v>
+        <v>-0.0737527170029693</v>
       </c>
       <c r="T30" t="n">
-        <v>-0.0186169799009149</v>
+        <v>-0.0256350914030362</v>
       </c>
       <c r="U30" t="n">
-        <v>0</v>
+        <v>-0.0620649059727352</v>
       </c>
       <c r="V30" t="n">
-        <v>-0.0208322214997017</v>
+        <v>-0.025698983412964</v>
       </c>
       <c r="W30" t="n">
-        <v>-0.0154334637361122</v>
+        <v>-0.028994862613142</v>
       </c>
       <c r="X30" t="n">
-        <v>-0.0787621371260853</v>
+        <v>-0.1433382646432998</v>
       </c>
       <c r="Y30" t="n">
-        <v>-0.0196849059739982</v>
+        <v>-0.0120270496173743</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>30-21377172</t>
+          <t>30-y2314105</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.1172758008439972</v>
+        <v>-0.0364126224532601</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.9925090340633842</v>
+        <v>-2.34518772820184</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.0928164886063495</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.1084279012113507</v>
+        <v>-0.061360676932035</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.0188830547014596</v>
+        <v>-0.1517741877928331</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.2873996272203751</v>
+        <v>-0.0634981296955543</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.9777528916703392</v>
+        <v>-0.8083577369367915</v>
       </c>
       <c r="I31" t="n">
-        <v>-0.0139224732909524</v>
+        <v>-0.1360556253784648</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.1000059627966426</v>
+        <v>-0.0103036998235217</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.1947964706792425</v>
+        <v>-0.1530353631928751</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.08156981225411471</v>
+        <v>-0.0960940067316356</v>
       </c>
       <c r="M31" t="n">
-        <v>-1.572128215373128</v>
+        <v>-2.508016463306971</v>
       </c>
       <c r="N31" t="n">
-        <v>-0.0099886126364111</v>
+        <v>-0.5259679288898809</v>
       </c>
       <c r="O31" t="n">
-        <v>-0.0419521730729267</v>
+        <v>-0.0403836922849106</v>
       </c>
       <c r="P31" t="n">
-        <v>-0.0618315130200671</v>
+        <v>-0.07100461378385731</v>
       </c>
       <c r="Q31" t="n">
-        <v>-0.1309116062765948</v>
+        <v>-0.0303944424966613</v>
       </c>
       <c r="R31" t="n">
-        <v>-0.73680941534172</v>
+        <v>-0.126455835976965</v>
       </c>
       <c r="S31" t="n">
-        <v>-0.0269487106507198</v>
+        <v>-0.037970436571735</v>
       </c>
       <c r="T31" t="n">
-        <v>-0.047595621167344</v>
+        <v>-0.0715483793723239</v>
       </c>
       <c r="U31" t="n">
-        <v>-0.0118341022973095</v>
+        <v>-0.1284982390512838</v>
       </c>
       <c r="V31" t="n">
-        <v>-0.1531862094332308</v>
+        <v>-0.0664600427747387</v>
       </c>
       <c r="W31" t="n">
-        <v>-0.1291350207952104</v>
+        <v>-0.1420092275677147</v>
       </c>
       <c r="X31" t="n">
-        <v>0</v>
+        <v>-0.0269704918703539</v>
       </c>
       <c r="Y31" t="n">
-        <v>-0.0682459530851356</v>
+        <v>-0.1937262588019832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>